<commit_message>
Do not shift freight to ships in NV, where there are no freight ships
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-nevada\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4D269-1906-40C9-9438-66386A9FA2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51BE1A3-5A14-4E6F-BBE7-B3F645EAA1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
+    <workbookView xWindow="1710" yWindow="930" windowWidth="24510" windowHeight="14880" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -966,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
updated RTMF to take out mode shifting
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Virginia\Models\eps-virginia\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Nevada\NV_model\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7159C0C3-3BCF-4B40-A1A8-AC29F16AE72E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" activeTab="1"/>
+    <workbookView xWindow="4365" yWindow="600" windowWidth="24435" windowHeight="15630" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,7 +529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -658,14 +659,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +884,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -966,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -977,7 +980,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="6">
         <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>